<commit_message>
fixed sourcing for first stage
</commit_message>
<xml_diff>
--- a/Documentation/Hardware/First_Stage/First_Stage_Sourcing.xlsx
+++ b/Documentation/Hardware/First_Stage/First_Stage_Sourcing.xlsx
@@ -5,10 +5,10 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="B:\ToPush\First_Stage\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="B:\Spikes\Documentation\Hardware\First_Stage\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{35E94EED-16DB-4B13-9CBF-74486954BD1B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D943AC0F-2533-494D-8938-B229CCE814DF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="30612" yWindow="-108" windowWidth="30936" windowHeight="18696" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="116" uniqueCount="82">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="116" uniqueCount="81">
   <si>
     <t>QTY</t>
   </si>
@@ -80,12 +80,6 @@
     <t>Panelmount, 6mm hole</t>
   </si>
   <si>
-    <t>Total Cost</t>
-  </si>
-  <si>
-    <t>Cost p.P. $</t>
-  </si>
-  <si>
     <t>Link Vendor</t>
   </si>
   <si>
@@ -282,6 +276,9 @@
   </si>
   <si>
     <t>Voltage Regulator Bracket Right</t>
+  </si>
+  <si>
+    <t>Hex-Grill</t>
   </si>
 </sst>
 </file>
@@ -357,7 +354,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
@@ -373,6 +370,7 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -654,10 +652,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:J21"/>
+  <dimension ref="A1:J20"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
-      <selection activeCell="C22" sqref="C22"/>
+    <sheetView tabSelected="1" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
+      <selection activeCell="A8" sqref="A8:I8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
@@ -675,13 +673,13 @@
   <sheetData>
     <row r="1" spans="1:10" x14ac:dyDescent="0.4">
       <c r="A1" s="1" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
     </row>
     <row r="2" spans="1:10" x14ac:dyDescent="0.4">
       <c r="D2" s="3"/>
     </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.4">
+    <row r="3" spans="1:10" s="9" customFormat="1" x14ac:dyDescent="0.4">
       <c r="A3" s="2" t="s">
         <v>0</v>
       </c>
@@ -701,7 +699,7 @@
         <v>4</v>
       </c>
       <c r="G3" s="2" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="H3" s="2" t="s">
         <v>5</v>
@@ -709,40 +707,34 @@
       <c r="I3" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="J3" s="2" t="s">
-        <v>15</v>
-      </c>
     </row>
     <row r="4" spans="1:10" x14ac:dyDescent="0.4">
       <c r="A4">
         <v>1</v>
       </c>
       <c r="B4" t="s">
+        <v>17</v>
+      </c>
+      <c r="C4" t="s">
+        <v>18</v>
+      </c>
+      <c r="D4" t="s">
+        <v>20</v>
+      </c>
+      <c r="E4" t="s">
         <v>19</v>
       </c>
-      <c r="C4" t="s">
-        <v>20</v>
-      </c>
-      <c r="D4" t="s">
-        <v>22</v>
-      </c>
-      <c r="E4" t="s">
+      <c r="F4" t="s">
+        <v>18</v>
+      </c>
+      <c r="G4" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="H4" s="4" t="s">
         <v>21</v>
       </c>
-      <c r="F4" t="s">
-        <v>20</v>
-      </c>
-      <c r="G4" s="4" t="s">
-        <v>18</v>
-      </c>
-      <c r="H4" s="4" t="s">
-        <v>23</v>
-      </c>
       <c r="I4" t="s">
-        <v>21</v>
-      </c>
-      <c r="J4">
-        <v>265.58</v>
+        <v>19</v>
       </c>
     </row>
     <row r="5" spans="1:10" x14ac:dyDescent="0.4">
@@ -750,31 +742,28 @@
         <v>1</v>
       </c>
       <c r="B5" t="s">
+        <v>24</v>
+      </c>
+      <c r="C5" t="s">
+        <v>25</v>
+      </c>
+      <c r="D5" t="s">
+        <v>20</v>
+      </c>
+      <c r="E5" t="s">
+        <v>19</v>
+      </c>
+      <c r="F5" t="s">
+        <v>25</v>
+      </c>
+      <c r="G5" s="6" t="s">
         <v>26</v>
       </c>
-      <c r="C5" t="s">
+      <c r="H5" s="4" t="s">
         <v>27</v>
       </c>
-      <c r="D5" t="s">
-        <v>22</v>
-      </c>
-      <c r="E5" t="s">
-        <v>21</v>
-      </c>
-      <c r="F5" t="s">
-        <v>27</v>
-      </c>
-      <c r="G5" s="6" t="s">
-        <v>28</v>
-      </c>
-      <c r="H5" s="4" t="s">
-        <v>29</v>
-      </c>
       <c r="I5" t="s">
-        <v>21</v>
-      </c>
-      <c r="J5">
-        <v>126.43</v>
+        <v>19</v>
       </c>
     </row>
     <row r="6" spans="1:10" x14ac:dyDescent="0.4">
@@ -782,64 +771,60 @@
         <v>2</v>
       </c>
       <c r="B6" t="s">
+        <v>29</v>
+      </c>
+      <c r="C6" s="7" t="s">
+        <v>28</v>
+      </c>
+      <c r="D6" t="s">
+        <v>30</v>
+      </c>
+      <c r="E6" t="s">
+        <v>19</v>
+      </c>
+      <c r="F6" s="7" t="s">
+        <v>28</v>
+      </c>
+      <c r="G6" s="4" t="s">
         <v>31</v>
       </c>
-      <c r="C6" s="7" t="s">
-        <v>30</v>
-      </c>
-      <c r="D6" t="s">
+      <c r="H6" s="4" t="s">
         <v>32</v>
       </c>
-      <c r="E6" t="s">
-        <v>21</v>
-      </c>
-      <c r="F6" s="7" t="s">
-        <v>30</v>
-      </c>
-      <c r="G6" s="4" t="s">
-        <v>33</v>
-      </c>
-      <c r="H6" s="4" t="s">
-        <v>34</v>
-      </c>
       <c r="I6" t="s">
-        <v>21</v>
-      </c>
-      <c r="J6" s="7">
-        <v>7.75</v>
-      </c>
+        <v>19</v>
+      </c>
+      <c r="J6" s="7"/>
     </row>
     <row r="7" spans="1:10" x14ac:dyDescent="0.4">
       <c r="A7">
         <v>2</v>
       </c>
       <c r="B7" t="s">
+        <v>33</v>
+      </c>
+      <c r="C7" s="7" t="s">
+        <v>34</v>
+      </c>
+      <c r="D7" t="s">
+        <v>37</v>
+      </c>
+      <c r="E7" t="s">
+        <v>19</v>
+      </c>
+      <c r="F7" s="7" t="s">
+        <v>34</v>
+      </c>
+      <c r="G7" s="4" t="s">
         <v>35</v>
       </c>
-      <c r="C7" s="7" t="s">
+      <c r="H7" s="4" t="s">
         <v>36</v>
       </c>
-      <c r="D7" t="s">
-        <v>39</v>
-      </c>
-      <c r="E7" t="s">
-        <v>21</v>
-      </c>
-      <c r="F7" s="7" t="s">
-        <v>36</v>
-      </c>
-      <c r="G7" s="4" t="s">
-        <v>37</v>
-      </c>
-      <c r="H7" s="4" t="s">
-        <v>38</v>
-      </c>
       <c r="I7" t="s">
-        <v>21</v>
-      </c>
-      <c r="J7" s="7">
-        <v>6.45</v>
-      </c>
+        <v>19</v>
+      </c>
+      <c r="J7" s="7"/>
     </row>
     <row r="8" spans="1:10" x14ac:dyDescent="0.4">
       <c r="A8">
@@ -861,48 +846,42 @@
         <v>11</v>
       </c>
       <c r="G8" s="4" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="H8" s="4" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="I8" t="s">
         <v>7</v>
       </c>
-      <c r="J8">
-        <v>12.15</v>
-      </c>
     </row>
     <row r="9" spans="1:10" x14ac:dyDescent="0.4">
       <c r="A9">
         <v>1</v>
       </c>
       <c r="B9" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="C9" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="D9" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="E9" t="s">
+        <v>38</v>
+      </c>
+      <c r="F9" t="s">
+        <v>41</v>
+      </c>
+      <c r="G9" s="6" t="s">
+        <v>39</v>
+      </c>
+      <c r="H9" s="4" t="s">
         <v>40</v>
       </c>
-      <c r="F9" t="s">
-        <v>43</v>
-      </c>
-      <c r="G9" s="6" t="s">
-        <v>41</v>
-      </c>
-      <c r="H9" s="4" t="s">
-        <v>42</v>
-      </c>
       <c r="I9" t="s">
-        <v>40</v>
-      </c>
-      <c r="J9">
-        <v>74.239999999999995</v>
+        <v>38</v>
       </c>
     </row>
     <row r="10" spans="1:10" x14ac:dyDescent="0.4">
@@ -910,31 +889,28 @@
         <v>1</v>
       </c>
       <c r="B10" t="s">
+        <v>46</v>
+      </c>
+      <c r="C10" t="s">
+        <v>50</v>
+      </c>
+      <c r="D10" t="s">
+        <v>54</v>
+      </c>
+      <c r="E10" t="s">
+        <v>47</v>
+      </c>
+      <c r="F10" t="s">
+        <v>49</v>
+      </c>
+      <c r="G10" s="4" t="s">
+        <v>44</v>
+      </c>
+      <c r="H10" s="4" t="s">
         <v>48</v>
       </c>
-      <c r="C10" t="s">
-        <v>52</v>
-      </c>
-      <c r="D10" t="s">
-        <v>56</v>
-      </c>
-      <c r="E10" t="s">
-        <v>49</v>
-      </c>
-      <c r="F10" t="s">
-        <v>51</v>
-      </c>
-      <c r="G10" s="4" t="s">
-        <v>46</v>
-      </c>
-      <c r="H10" s="4" t="s">
-        <v>50</v>
-      </c>
       <c r="I10" t="s">
-        <v>47</v>
-      </c>
-      <c r="J10">
-        <v>11.99</v>
+        <v>45</v>
       </c>
     </row>
     <row r="11" spans="1:10" x14ac:dyDescent="0.4">
@@ -942,31 +918,28 @@
         <v>1</v>
       </c>
       <c r="B11" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="C11" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="D11" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="E11" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="F11" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="G11" s="4" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="H11" s="4" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="I11" t="s">
-        <v>47</v>
-      </c>
-      <c r="J11">
-        <v>11.99</v>
+        <v>45</v>
       </c>
     </row>
     <row r="12" spans="1:10" x14ac:dyDescent="0.4">
@@ -974,31 +947,28 @@
         <v>1</v>
       </c>
       <c r="B12" t="s">
+        <v>56</v>
+      </c>
+      <c r="C12" t="s">
+        <v>57</v>
+      </c>
+      <c r="D12" t="s">
         <v>58</v>
       </c>
-      <c r="C12" t="s">
+      <c r="E12" t="s">
         <v>59</v>
       </c>
-      <c r="D12" t="s">
-        <v>60</v>
-      </c>
-      <c r="E12" t="s">
+      <c r="F12" t="s">
         <v>61</v>
       </c>
-      <c r="F12" t="s">
+      <c r="G12" s="4" t="s">
+        <v>62</v>
+      </c>
+      <c r="H12" s="8" t="s">
         <v>63</v>
       </c>
-      <c r="G12" s="4" t="s">
-        <v>64</v>
-      </c>
-      <c r="H12" s="8" t="s">
-        <v>65</v>
-      </c>
       <c r="I12" t="s">
-        <v>47</v>
-      </c>
-      <c r="J12">
-        <v>8.99</v>
+        <v>45</v>
       </c>
     </row>
     <row r="13" spans="1:10" x14ac:dyDescent="0.4">
@@ -1006,31 +976,28 @@
         <v>1</v>
       </c>
       <c r="B13" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="C13" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="D13" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="E13" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="F13" t="s">
+        <v>61</v>
+      </c>
+      <c r="G13" s="4" t="s">
+        <v>64</v>
+      </c>
+      <c r="H13" s="8" t="s">
         <v>63</v>
       </c>
-      <c r="G13" s="4" t="s">
-        <v>66</v>
-      </c>
-      <c r="H13" s="8" t="s">
-        <v>65</v>
-      </c>
       <c r="I13" t="s">
-        <v>47</v>
-      </c>
-      <c r="J13">
-        <v>12.69</v>
+        <v>45</v>
       </c>
     </row>
     <row r="14" spans="1:10" x14ac:dyDescent="0.4">
@@ -1038,31 +1005,28 @@
         <v>1</v>
       </c>
       <c r="B14" t="s">
+        <v>69</v>
+      </c>
+      <c r="C14" t="s">
+        <v>73</v>
+      </c>
+      <c r="D14" t="s">
+        <v>66</v>
+      </c>
+      <c r="E14" t="s">
+        <v>70</v>
+      </c>
+      <c r="F14" t="s">
+        <v>61</v>
+      </c>
+      <c r="G14" s="4" t="s">
         <v>71</v>
       </c>
-      <c r="C14" t="s">
-        <v>75</v>
-      </c>
-      <c r="D14" t="s">
-        <v>68</v>
-      </c>
-      <c r="E14" t="s">
-        <v>72</v>
-      </c>
-      <c r="F14" t="s">
+      <c r="H14" s="8" t="s">
         <v>63</v>
       </c>
-      <c r="G14" s="4" t="s">
-        <v>73</v>
-      </c>
-      <c r="H14" s="8" t="s">
-        <v>65</v>
-      </c>
       <c r="I14" t="s">
-        <v>47</v>
-      </c>
-      <c r="J14">
-        <v>11.69</v>
+        <v>45</v>
       </c>
     </row>
     <row r="15" spans="1:10" x14ac:dyDescent="0.4">
@@ -1070,31 +1034,28 @@
         <v>1</v>
       </c>
       <c r="B15" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="C15" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="D15" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="E15" t="s">
+        <v>70</v>
+      </c>
+      <c r="F15" t="s">
+        <v>61</v>
+      </c>
+      <c r="G15" s="4" t="s">
         <v>72</v>
       </c>
-      <c r="F15" t="s">
+      <c r="H15" s="8" t="s">
         <v>63</v>
       </c>
-      <c r="G15" s="4" t="s">
-        <v>74</v>
-      </c>
-      <c r="H15" s="8" t="s">
-        <v>65</v>
-      </c>
       <c r="I15" t="s">
-        <v>47</v>
-      </c>
-      <c r="J15">
-        <v>11.69</v>
+        <v>45</v>
       </c>
     </row>
     <row r="16" spans="1:10" x14ac:dyDescent="0.4">
@@ -1102,55 +1063,57 @@
         <v>1</v>
       </c>
       <c r="B16" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="C16" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="G16" s="4"/>
       <c r="H16" s="4"/>
       <c r="J16" s="5"/>
     </row>
-    <row r="17" spans="1:10" x14ac:dyDescent="0.4">
+    <row r="17" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A17">
         <v>1</v>
       </c>
       <c r="B17" t="s">
+        <v>75</v>
+      </c>
+      <c r="C17" t="s">
         <v>77</v>
       </c>
-      <c r="C17" t="s">
+    </row>
+    <row r="18" spans="1:3" x14ac:dyDescent="0.4">
+      <c r="A18">
+        <v>1</v>
+      </c>
+      <c r="B18" t="s">
+        <v>75</v>
+      </c>
+      <c r="C18" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="19" spans="1:3" x14ac:dyDescent="0.4">
+      <c r="A19">
+        <v>1</v>
+      </c>
+      <c r="B19" t="s">
+        <v>75</v>
+      </c>
+      <c r="C19" t="s">
         <v>79</v>
       </c>
     </row>
-    <row r="18" spans="1:10" x14ac:dyDescent="0.4">
-      <c r="A18">
-        <v>1</v>
-      </c>
-      <c r="B18" t="s">
-        <v>77</v>
-      </c>
-      <c r="C18" t="s">
+    <row r="20" spans="1:3" x14ac:dyDescent="0.4">
+      <c r="A20">
+        <v>2</v>
+      </c>
+      <c r="B20" t="s">
+        <v>75</v>
+      </c>
+      <c r="C20" t="s">
         <v>80</v>
-      </c>
-    </row>
-    <row r="19" spans="1:10" x14ac:dyDescent="0.4">
-      <c r="A19">
-        <v>1</v>
-      </c>
-      <c r="B19" t="s">
-        <v>77</v>
-      </c>
-      <c r="C19" t="s">
-        <v>81</v>
-      </c>
-    </row>
-    <row r="21" spans="1:10" x14ac:dyDescent="0.4">
-      <c r="I21" t="s">
-        <v>14</v>
-      </c>
-      <c r="J21">
-        <f>A4*J4+A5*J5+A10*J10+A7*J7+A8*J8+A9*J9+A6*J6+A11*J11+A12*J12+A13*J13+A14*J14+A15*J15+A16*J16</f>
-        <v>575.84000000000015</v>
       </c>
     </row>
   </sheetData>

</xml_diff>